<commit_message>
pipeline ran - 26-08-2025
</commit_message>
<xml_diff>
--- a/data_validation/HuggingFace/2025/08/23/validation_report.xlsx
+++ b/data_validation/HuggingFace/2025/08/23/validation_report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91880\Documents\Career\wilp\semester-2\DMML\Assignment\DMML-Assignment\4. Data Validation\HuggingFace\2025\08\23\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91880\Documents\Career\wilp\semester-2\DMML\Assignment\DMML-Assignment\data_validation\HuggingFace\2025\08\23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBA433A-8D92-4103-9795-4BD984F61414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121F2842-8016-4767-93B2-87845D9D74AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22476" yWindow="1020" windowWidth="21600" windowHeight="11292" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4185" yWindow="3315" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -469,7 +469,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,13 +500,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -526,7 +526,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -540,7 +540,7 @@
         <v>5</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -568,7 +568,7 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>

</xml_diff>